<commit_message>
updated version with star!
</commit_message>
<xml_diff>
--- a/Danfoss Heating system/Assets/data.xlsx
+++ b/Danfoss Heating system/Assets/data.xlsx
@@ -7055,7 +7055,7 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="AG3" s="0">
-        <x:v>35</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="AH3" s="0">
         <x:v>0</x:v>
@@ -7064,7 +7064,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="AJ3" s="0">
-        <x:v>1.4</x:v>
+        <x:v>1.2</x:v>
       </x:c>
       <x:c r="AK3" s="0">
         <x:v>1</x:v>
@@ -7129,16 +7129,16 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="AG4" s="0">
-        <x:v>35</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="AH4" s="0">
-        <x:v>3994.7904</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AI4" s="0">
-        <x:v>2304</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AJ4" s="0">
-        <x:v>1.26</x:v>
+        <x:v>1.08</x:v>
       </x:c>
       <x:c r="AK4" s="0">
         <x:v>1</x:v>
@@ -7197,13 +7197,13 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="AE5" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="AF5" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="AG5" s="0">
-        <x:v>55</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AH5" s="0">
         <x:v>0</x:v>
@@ -7212,10 +7212,10 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="AJ5" s="0">
-        <x:v>4.4</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AK5" s="0">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -7327,25 +7327,25 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="AE7" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="AF7" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="AG7" s="0">
-        <x:v>35</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AH7" s="0">
-        <x:v>2500</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AI7" s="0">
-        <x:v>1075</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AJ7" s="0">
-        <x:v>1.75</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AK7" s="0">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -7383,13 +7383,13 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="AE8" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="AF8" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="AG8" s="0">
-        <x:v>75</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AH8" s="0">
         <x:v>0</x:v>
@@ -7398,10 +7398,10 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="AJ8" s="0">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AK8" s="0">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -7439,13 +7439,13 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="AE9" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="AF9" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="AG9" s="0">
-        <x:v>35</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AH9" s="0">
         <x:v>0</x:v>
@@ -7454,10 +7454,10 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="AJ9" s="0">
-        <x:v>1.26</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AK9" s="0">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -7495,13 +7495,13 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="AE10" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="AF10" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="AG10" s="0">
-        <x:v>55</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AH10" s="0">
         <x:v>0</x:v>
@@ -7510,10 +7510,10 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="AJ10" s="0">
-        <x:v>4.4</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="AK10" s="0">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>